<commit_message>
decode with test file results in *all* generic responses.
</commit_message>
<xml_diff>
--- a/Exp/MMI/ppl-batch_n.xlsx
+++ b/Exp/MMI/ppl-batch_n.xlsx
@@ -1595,6 +1595,43 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="" altLang="en-US"/>
+              <a:t>Perplexity vs bach_n</a:t>
+            </a:r>
+            <a:endParaRPr lang="" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1950,6 +1987,43 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="" altLang="en-US"/>
+                  <a:t>batch_n</a:t>
+                </a:r>
+                <a:endParaRPr lang="" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2013,8 +2087,45 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="" altLang="en-US"/>
+                  <a:t>PPL</a:t>
+                </a:r>
+                <a:endParaRPr lang="" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3864,16 +3975,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>300355</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>71755</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>651510</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>77470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>492760</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>149860</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>158115</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3881,7 +3992,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3864610" y="1043305"/>
+        <a:off x="5587365" y="887095"/>
         <a:ext cx="6364605" cy="4126230"/>
       </xdr:xfrm>
       <a:graphic>
@@ -4523,7 +4634,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B5" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="D5" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>

</xml_diff>